<commit_message>
changed int to unsigned long long, implemented tests for fibonacci and fibonacciSum
</commit_message>
<xml_diff>
--- a/fibonacciUpTo50.xlsx
+++ b/fibonacciUpTo50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\total\Documents\GitHub\SE282-assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FA6A783-29D1-4F81-A606-5E39B1440122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C158042C-8834-422E-AB75-FA918848B5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{E0ED11BD-3B20-411D-9F1C-C94B92CB4256}"/>
   </bookViews>
@@ -68,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +93,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -106,12 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,13 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBD557C-4721-437C-8C09-A984D251B6DA}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -533,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B6:B52" si="0">$B5 + $B6</f>
+        <f t="shared" ref="B7:B70" si="0">$B5 + $B6</f>
         <v>5</v>
       </c>
       <c r="C7" s="4">
@@ -1124,6 +1135,656 @@
       <c r="C52">
         <f>SUM($B$2:$B52)</f>
         <v>32951280098</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>20365011074</v>
+      </c>
+      <c r="C53">
+        <f>SUM($B$2:$B53)</f>
+        <v>53316291172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>32951280099</v>
+      </c>
+      <c r="C54">
+        <f>SUM($B$2:$B54)</f>
+        <v>86267571271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>53316291173</v>
+      </c>
+      <c r="C55">
+        <f>SUM($B$2:$B55)</f>
+        <v>139583862444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>86267571272</v>
+      </c>
+      <c r="C56">
+        <f>SUM($B$2:$B56)</f>
+        <v>225851433716</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>139583862445</v>
+      </c>
+      <c r="C57">
+        <f>SUM($B$2:$B57)</f>
+        <v>365435296161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>225851433717</v>
+      </c>
+      <c r="C58">
+        <f>SUM($B$2:$B58)</f>
+        <v>591286729878</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>365435296162</v>
+      </c>
+      <c r="C59">
+        <f>SUM($B$2:$B59)</f>
+        <v>956722026040</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>591286729879</v>
+      </c>
+      <c r="C60">
+        <f>SUM($B$2:$B60)</f>
+        <v>1548008755919</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>956722026041</v>
+      </c>
+      <c r="C61">
+        <f>SUM($B$2:$B61)</f>
+        <v>2504730781960</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>1548008755920</v>
+      </c>
+      <c r="C62">
+        <f>SUM($B$2:$B62)</f>
+        <v>4052739537880</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>2504730781961</v>
+      </c>
+      <c r="C63">
+        <f>SUM($B$2:$B63)</f>
+        <v>6557470319841</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>4052739537881</v>
+      </c>
+      <c r="C64">
+        <f>SUM($B$2:$B64)</f>
+        <v>10610209857722</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>6557470319842</v>
+      </c>
+      <c r="C65">
+        <f>SUM($B$2:$B65)</f>
+        <v>17167680177564</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>10610209857723</v>
+      </c>
+      <c r="C66">
+        <f>SUM($B$2:$B66)</f>
+        <v>27777890035287</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>17167680177565</v>
+      </c>
+      <c r="C67">
+        <f>SUM($B$2:$B67)</f>
+        <v>44945570212852</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>27777890035288</v>
+      </c>
+      <c r="C68">
+        <f>SUM($B$2:$B68)</f>
+        <v>72723460248140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>44945570212853</v>
+      </c>
+      <c r="C69">
+        <f>SUM($B$2:$B69)</f>
+        <v>117669030460993</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>72723460248141</v>
+      </c>
+      <c r="C70">
+        <f>SUM($B$2:$B70)</f>
+        <v>190392490709134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <f t="shared" ref="B71:B102" si="1">$B69 + $B70</f>
+        <v>117669030460994</v>
+      </c>
+      <c r="C71">
+        <f>SUM($B$2:$B71)</f>
+        <v>308061521170128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>190392490709135</v>
+      </c>
+      <c r="C72">
+        <f>SUM($B$2:$B72)</f>
+        <v>498454011879263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>308061521170129</v>
+      </c>
+      <c r="C73">
+        <f>SUM($B$2:$B73)</f>
+        <v>806515533049392</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>498454011879264</v>
+      </c>
+      <c r="C74">
+        <f>SUM($B$2:$B74)</f>
+        <v>1304969544928656</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>806515533049393</v>
+      </c>
+      <c r="C75">
+        <f>SUM($B$2:$B75)</f>
+        <v>2111485077978049</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>1304969544928657</v>
+      </c>
+      <c r="C76">
+        <f>SUM($B$2:$B76)</f>
+        <v>3416454622906706</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>2111485077978050</v>
+      </c>
+      <c r="C77">
+        <f>SUM($B$2:$B77)</f>
+        <v>5527939700884756</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>3416454622906707</v>
+      </c>
+      <c r="C78">
+        <f>SUM($B$2:$B78)</f>
+        <v>8944394323791463</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>5527939700884757</v>
+      </c>
+      <c r="C79">
+        <f>SUM($B$2:$B79)</f>
+        <v>1.447233402467622E+16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>8944394323791464</v>
+      </c>
+      <c r="C80">
+        <f>SUM($B$2:$B80)</f>
+        <v>2.3416728348467684E+16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>1.447233402467622E+16</v>
+      </c>
+      <c r="C81">
+        <f>SUM($B$2:$B81)</f>
+        <v>3.7889062373143904E+16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>2.3416728348467684E+16</v>
+      </c>
+      <c r="C82">
+        <f>SUM($B$2:$B82)</f>
+        <v>6.1305790721611584E+16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>3.7889062373143904E+16</v>
+      </c>
+      <c r="C83">
+        <f>SUM($B$2:$B83)</f>
+        <v>9.9194853094755488E+16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>6.1305790721611584E+16</v>
+      </c>
+      <c r="C84">
+        <f>SUM($B$2:$B84)</f>
+        <v>1.6050064381636707E+17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>9.9194853094755488E+16</v>
+      </c>
+      <c r="C85">
+        <f>SUM($B$2:$B85)</f>
+        <v>2.5969549691112256E+17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>1.6050064381636707E+17</v>
+      </c>
+      <c r="C86">
+        <f>SUM($B$2:$B86)</f>
+        <v>4.2019614072748966E+17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>2.5969549691112256E+17</v>
+      </c>
+      <c r="C87">
+        <f>SUM($B$2:$B87)</f>
+        <v>6.7989163763861222E+17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>4.2019614072748966E+17</v>
+      </c>
+      <c r="C88">
+        <f>SUM($B$2:$B88)</f>
+        <v>1.1000877783661019E+18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>6.7989163763861222E+17</v>
+      </c>
+      <c r="C89">
+        <f>SUM($B$2:$B89)</f>
+        <v>1.779979416004714E+18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>1.1000877783661019E+18</v>
+      </c>
+      <c r="C90">
+        <f>SUM($B$2:$B90)</f>
+        <v>2.880067194370816E+18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>1.779979416004714E+18</v>
+      </c>
+      <c r="C91">
+        <f>SUM($B$2:$B91)</f>
+        <v>4.6600466103755305E+18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>2.880067194370816E+18</v>
+      </c>
+      <c r="C92">
+        <f>SUM($B$2:$B92)</f>
+        <v>7.5401138047463465E+18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>91</v>
+      </c>
+      <c r="B93" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6600466103755305E+18</v>
+      </c>
+      <c r="C93" s="2">
+        <f>SUM($B$2:$B93)</f>
+        <v>1.2200160415121877E+19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>92</v>
+      </c>
+      <c r="B94" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5401138047463465E+18</v>
+      </c>
+      <c r="C94" s="5">
+        <f>SUM($B$2:$B94)</f>
+        <v>1.9740274219868226E+19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>93</v>
+      </c>
+      <c r="B95" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2200160415121877E+19</v>
+      </c>
+      <c r="C95" s="5">
+        <f>SUM($B$2:$B95)</f>
+        <v>3.19404346349901E+19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>94</v>
+      </c>
+      <c r="B96" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9740274219868226E+19</v>
+      </c>
+      <c r="C96" s="5">
+        <f>SUM($B$2:$B96)</f>
+        <v>5.1680708854858326E+19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>95</v>
+      </c>
+      <c r="B97" s="5">
+        <f t="shared" si="1"/>
+        <v>3.19404346349901E+19</v>
+      </c>
+      <c r="C97" s="5">
+        <f>SUM($B$2:$B97)</f>
+        <v>8.3621143489848426E+19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>96</v>
+      </c>
+      <c r="B98" s="5">
+        <f t="shared" si="1"/>
+        <v>5.1680708854858326E+19</v>
+      </c>
+      <c r="C98" s="5">
+        <f>SUM($B$2:$B98)</f>
+        <v>1.3530185234470676E+20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>97</v>
+      </c>
+      <c r="B99" s="5">
+        <f t="shared" si="1"/>
+        <v>8.3621143489848426E+19</v>
+      </c>
+      <c r="C99" s="5">
+        <f>SUM($B$2:$B99)</f>
+        <v>2.189229958345552E+20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>98</v>
+      </c>
+      <c r="B100" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3530185234470676E+20</v>
+      </c>
+      <c r="C100" s="5">
+        <f>SUM($B$2:$B100)</f>
+        <v>3.54224848179262E+20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>99</v>
+      </c>
+      <c r="B101" s="5">
+        <f t="shared" si="1"/>
+        <v>2.189229958345552E+20</v>
+      </c>
+      <c r="C101" s="5">
+        <f>SUM($B$2:$B101)</f>
+        <v>5.731478440138172E+20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>100</v>
+      </c>
+      <c r="B102" s="5">
+        <f t="shared" si="1"/>
+        <v>3.54224848179262E+20</v>
+      </c>
+      <c r="C102" s="5">
+        <f>SUM($B$2:$B102)</f>
+        <v>9.273726921930792E+20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>